<commit_message>
MeleeSecondSkill 수정, 기획 문서 수정
1. PlayerCtrl.cs
- isMeleeSecondSkilled 변수 추가
- GainHealth 함수 추가

2. PlayerBulletBasic.cs
- totalDamageDealt 변수 추가,
- OnTriggerEnter에 totalDamageDealt를 증가시키는 로직 추가

3. MeleeSkillSecond.cs 수정

4. MeleeWeaponThird 무기 이름 및 설명 변경

5. UDP_PlayerWeapon 기획문서의 모든 총알 속도 변경

6. UDP_PlayerWeapon 기획문서의 근거리 주포 관련 설명 변경
</commit_message>
<xml_diff>
--- a/기획문서/UDP_PlayerWeapons.xlsx
+++ b/기획문서/UDP_PlayerWeapons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GithubProject\UDP\기획문서\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\UDP\기획문서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C529A0-8360-46B5-9951-758209D99313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B7B481-0065-475B-813F-18CAA9FB4A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{62910332-10B0-4234-AE16-77750EBC7CE9}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{62910332-10B0-4234-AE16-77750EBC7CE9}"/>
   </bookViews>
   <sheets>
     <sheet name="근거리" sheetId="4" r:id="rId1"/>
@@ -193,126 +193,285 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>폭발탄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>적에게 두 번의 데미지를 주는 탄환을 발사하는 주포입니다. 적중한 탄환은 2초 후 한 번 더 폭발하여, 탄환 피해량의 20%/30%/40%/50%만큼 추가 피해를 입힙니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최소 피해량: (10) + (10) + (15 + 7.5) + (20 + 10 + 10 + 5) = 87.5</t>
+  </si>
+  <si>
+    <t>적의 체력은 100~200, 4번~6번의 공격을 맞으면 적이 사망한다고 가정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">최대 피해량: (10) + (10) + (48 + 24) + ( 56 + 28 + 28 + 14) = 218 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방어막</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3초 동안 적의 공격을 막아주는 방어막을 생성합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5초 동안 적에게 입힌 피해만큼 내구도를 회복합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타오르는 힘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 중 24거리 이내의 적 포착 시 추적</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 중 반지름 20거리 이내의 적 포착 시 추적</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 중 28거리 이내의 적 포착 시 추적</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 중 32거리 이내의 적 포착 시 추적</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>폭발 범위 45</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>폭발 범위 50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 중 20거리 이내의 적 포착 시 폭발, 폭발 범위 35(반지름) 폭발에 휘말린 적은 폭발 방향으로 밀려남</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>폭발 범위 40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>포탄 속도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>코드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>melee_weapon_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>melee_weapon_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>melee_weapon_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>melee_weapon_4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>melee_skill_Q</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>melee_skill_E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본탄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>사슬 갈고리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>플레이어가 바라보는 방향으로 20/30/40/50의 속도로 사슬 갈고리를 던지며, 적중 시 플레이어가 60의 속도로 적중한 적에게 이동합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>폭발탄</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>산탄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>단일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격대상</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>포탄 타입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발당 피해량</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본이 되는 산탄 형태의 주포입니다. 레벨이 높아질수록 피해량과 발사되는 포탄의 수가 증가합니다.</t>
+  </si>
+  <si>
+    <t>적의 장갑과 외부 보호 장치를 부식시키는 탄환을 발사하는 주포입니다. 적중한 적에게 가하는 피해량이 3초 동안 50% 증가합니다.</t>
+  </si>
+  <si>
+    <t>특이사항/설명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>적에게 두 번의 데미지를 주는 탄환을 발사하는 주포입니다. 적중한 탄환은 2초 후 한 번 더 폭발하여, 탄환 피해량의 20%/30%/40%/50%만큼 추가 피해를 입힙니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>최소 피해량: (10) + (10) + (15 + 7.5) + (20 + 10 + 10 + 5) = 87.5</t>
-  </si>
-  <si>
-    <t>적의 체력은 100~200, 4번~6번의 공격을 맞으면 적이 사망한다고 가정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">최대 피해량: (10) + (10) + (48 + 24) + ( 56 + 28 + 28 + 14) = 218 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>방어막</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어가 바라보는 방향으로 사슬 갈고리를 던져, 적중 시 플레이어가 60의 속도로 적중한 적에게 이동합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>middle_weapon_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>middle_weapon_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>range_weapon_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>middle_weapon_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>middle_weapon_4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>range_weapon_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>range_weapon_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>range_weapon_4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>middle_skill_Q</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>middle_skill_E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>range_skill_Q</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>range_skill_E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다음에 사용하는 주포의 쿨타임을 1회 제거합니다.</t>
   </si>
   <si>
     <t>3초 동안 적의 공격을 막아주는 방어막을 생성합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>5초 동안 적에게 입힌 피해만큼 내구도를 회복합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>타오르는 힘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이동 중 24거리 이내의 적 포착 시 추적</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이동 중 반지름 20거리 이내의 적 포착 시 추적</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이동 중 28거리 이내의 적 포착 시 추적</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이동 중 32거리 이내의 적 포착 시 추적</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>폭발 범위 45</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>폭발 범위 50</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이동 중 20거리 이내의 적 포착 시 폭발, 폭발 범위 35(반지름) 폭발에 휘말린 적은 폭발 방향으로 밀려남</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>폭발 범위 40</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>포탄 속도</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>코드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>melee_weapon_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>melee_weapon_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>melee_weapon_3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>melee_weapon_4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>melee_skill_Q</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>melee_skill_E</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기본탄</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사슬 갈고리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>폭발탄</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>산탄</t>
+  </si>
+  <si>
+    <t>최대 체력의 20%를 회복합니다.</t>
+  </si>
+  <si>
+    <t>쿨타임(초)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동속도를 5초 동안 최고속도에 도달합니다. 긴급 탈출을 사용하는 동안 연료를 사용하지 않습니다</t>
+  </si>
+  <si>
+    <t>이동속도를 5초 동안 최고속도에 도달합니다. 긴급 탈출을 사용하는 동안 연료를 사용하지 않습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어 주변 20거리 이내 모든 적 포탄의 이동을 멈춥니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본 공격</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다크 매터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빨간 버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연속 공격</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>철갑소이탄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>근접 유도 어뢰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMP 자폭탄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플라즈마 광선</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4+(레벨)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3+(레벨)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2+(레벨)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10+(레벨)*10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7-(레벨)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -320,15 +479,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>공격대상</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>포탄 타입</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>발당 피해량</t>
+    <t>광역</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -336,165 +487,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>기본이 되는 산탄 형태의 주포입니다. 레벨이 높아질수록 피해량과 발사되는 포탄의 수가 증가합니다.</t>
-  </si>
-  <si>
-    <t>적의 장갑과 외부 보호 장치를 부식시키는 탄환을 발사하는 주포입니다. 적중한 적에게 가하는 피해량이 3초 동안 50% 증가합니다.</t>
-  </si>
-  <si>
-    <t>특이사항/설명</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>적에게 두 번의 데미지를 주는 탄환을 발사하는 주포입니다. 적중한 탄환은 2초 후 한 번 더 폭발하여, 탄환 피해량의 20%/30%/40%/50%만큼 추가 피해를 입힙니다.</t>
-  </si>
-  <si>
-    <t>플레이어가 바라보는 방향으로 사슬 갈고리를 던져, 적중 시 플레이어가 60의 속도로 적중한 적에게 이동합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>middle_weapon_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>middle_weapon_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>range_weapon_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>middle_weapon_3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>middle_weapon_4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>range_weapon_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>range_weapon_3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>range_weapon_4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>middle_skill_Q</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>middle_skill_E</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>range_skill_Q</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>range_skill_E</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>다음에 사용하는 주포의 쿨타임을 1회 제거합니다.</t>
-  </si>
-  <si>
-    <t>3초 동안 적의 공격을 막아주는 방어막을 생성합니다.</t>
-  </si>
-  <si>
-    <t>5초 동안 적에게 입힌 피해만큼 내구도를 회복합니다.</t>
-  </si>
-  <si>
-    <t>최대 체력의 20%를 회복합니다.</t>
-  </si>
-  <si>
-    <t>쿨타임(초)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이동속도를 5초 동안 최고속도에 도달합니다. 긴급 탈출을 사용하는 동안 연료를 사용하지 않습니다</t>
-  </si>
-  <si>
-    <t>이동속도를 5초 동안 최고속도에 도달합니다. 긴급 탈출을 사용하는 동안 연료를 사용하지 않습니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>플레이어 주변 20거리 이내 모든 적 포탄의 이동을 멈춥니다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기본 공격</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>다크 매터</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>빨간 버튼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>연속 공격</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>철갑소이탄</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>근접 유도 어뢰</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EMP 자폭탄</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>플라즈마 광선</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4+(레벨)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3+(레벨)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2+(레벨)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10+(레벨)*10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7-(레벨)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>단일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>광역</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일반</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -573,6 +565,14 @@
   </si>
   <si>
     <t>작성자: 5645866 구기현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>초강력 끈끈이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어가 바라보는 방향으로 20/30/40/50의 속도로 초강력 끈끈이를 던지며, 적중 시 플레이어가 60의 속도로 적중한 적에게 이동합니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -941,15 +941,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -974,9 +974,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -995,12 +992,36 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1009,27 +1030,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1367,28 +1367,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9994DB1-7A88-429D-9CFE-E67689A4F62A}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="2" max="2" width="15.625" customWidth="1"/>
     <col min="7" max="7" width="50.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
-        <v>133</v>
-      </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-    </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A3" s="35">
         <v>1</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="35">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E3" s="4">
         <v>5</v>
@@ -1435,7 +1435,7 @@
       </c>
       <c r="H3" s="20"/>
     </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A4" s="36"/>
       <c r="B4" s="36"/>
       <c r="C4" s="4">
@@ -1449,7 +1449,7 @@
       <c r="G4" s="42"/>
       <c r="H4" s="20"/>
     </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="36"/>
       <c r="B5" s="36"/>
       <c r="C5" s="4">
@@ -1462,7 +1462,7 @@
       <c r="F5" s="36"/>
       <c r="G5" s="42"/>
     </row>
-    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A6" s="37"/>
       <c r="B6" s="37"/>
       <c r="C6" s="4">
@@ -1475,7 +1475,7 @@
       <c r="F6" s="37"/>
       <c r="G6" s="43"/>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A7" s="28">
         <v>2</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="35">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="E7" s="35">
         <v>5</v>
@@ -1498,7 +1498,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A8" s="28"/>
       <c r="B8" s="36"/>
       <c r="C8" s="36"/>
@@ -1507,9 +1507,9 @@
       <c r="F8" s="4">
         <v>5</v>
       </c>
-      <c r="G8" s="45"/>
-    </row>
-    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G8" s="46"/>
+    </row>
+    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A9" s="28"/>
       <c r="B9" s="36"/>
       <c r="C9" s="36"/>
@@ -1518,9 +1518,9 @@
       <c r="F9" s="4">
         <v>4</v>
       </c>
-      <c r="G9" s="45"/>
-    </row>
-    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G9" s="46"/>
+    </row>
+    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A10" s="28"/>
       <c r="B10" s="37"/>
       <c r="C10" s="37"/>
@@ -1529,20 +1529,20 @@
       <c r="F10" s="10">
         <v>3</v>
       </c>
-      <c r="G10" s="46"/>
-    </row>
-    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="47"/>
+    </row>
+    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A11" s="28">
         <v>3</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>35</v>
+        <v>132</v>
       </c>
       <c r="C11" s="35">
         <v>10</v>
       </c>
       <c r="D11" s="4">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E11" s="35">
         <v>1</v>
@@ -1551,15 +1551,15 @@
         <v>6</v>
       </c>
       <c r="G11" s="38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A12" s="28"/>
       <c r="B12" s="36"/>
       <c r="C12" s="36"/>
       <c r="D12" s="4">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="E12" s="36"/>
       <c r="F12" s="4">
@@ -1567,12 +1567,12 @@
       </c>
       <c r="G12" s="39"/>
     </row>
-    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A13" s="28"/>
       <c r="B13" s="36"/>
       <c r="C13" s="36"/>
       <c r="D13" s="4">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E13" s="36"/>
       <c r="F13" s="4">
@@ -1580,12 +1580,12 @@
       </c>
       <c r="G13" s="39"/>
     </row>
-    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A14" s="28"/>
       <c r="B14" s="37"/>
       <c r="C14" s="37"/>
       <c r="D14" s="10">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="4">
@@ -1593,18 +1593,18 @@
       </c>
       <c r="G14" s="40"/>
     </row>
-    <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A15" s="28">
         <v>4</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="4">
         <v>5</v>
       </c>
       <c r="D15" s="35">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E15" s="4">
         <v>4</v>
@@ -1613,10 +1613,10 @@
         <v>8</v>
       </c>
       <c r="G15" s="41" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A16" s="28"/>
       <c r="B16" s="36"/>
       <c r="C16" s="4">
@@ -1629,7 +1629,7 @@
       <c r="F16" s="36"/>
       <c r="G16" s="42"/>
     </row>
-    <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A17" s="28"/>
       <c r="B17" s="36"/>
       <c r="C17" s="4">
@@ -1642,7 +1642,7 @@
       <c r="F17" s="36"/>
       <c r="G17" s="42"/>
     </row>
-    <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A18" s="28"/>
       <c r="B18" s="37"/>
       <c r="C18" s="4">
@@ -1655,12 +1655,12 @@
       <c r="F18" s="37"/>
       <c r="G18" s="43"/>
       <c r="H18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A19" s="44" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B19" s="44"/>
       <c r="C19" s="44"/>
@@ -1669,10 +1669,10 @@
       <c r="F19" s="44"/>
       <c r="G19" s="44"/>
       <c r="H19" s="20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
@@ -1687,18 +1687,18 @@
       <c r="F20" s="30"/>
       <c r="G20" s="31"/>
       <c r="H20" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A21" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D21" s="33"/>
       <c r="E21" s="33"/>
@@ -1708,15 +1708,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D22" s="33"/>
       <c r="E22" s="33"/>
@@ -1764,28 +1764,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38EF9496-DE58-419F-893B-F291F26CE53B}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="2" max="2" width="15.625" customWidth="1"/>
     <col min="7" max="7" width="45.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
-        <v>132</v>
-      </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1808,74 +1808,74 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A3" s="35">
         <v>1</v>
       </c>
-      <c r="B3" s="57" t="s">
-        <v>97</v>
+      <c r="B3" s="56" t="s">
+        <v>95</v>
       </c>
       <c r="C3" s="6">
         <v>25</v>
       </c>
       <c r="D3" s="35">
-        <v>25</v>
-      </c>
-      <c r="E3" s="57">
+        <v>75</v>
+      </c>
+      <c r="E3" s="56">
         <v>1</v>
       </c>
-      <c r="F3" s="60">
+      <c r="F3" s="59">
         <v>1</v>
       </c>
-      <c r="G3" s="60" t="s">
+      <c r="G3" s="59" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A4" s="36"/>
-      <c r="B4" s="58"/>
+      <c r="B4" s="57"/>
       <c r="C4" s="6">
         <v>35</v>
       </c>
       <c r="D4" s="36"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="58"/>
-    </row>
-    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="57"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="57"/>
+    </row>
+    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="36"/>
-      <c r="B5" s="58"/>
+      <c r="B5" s="57"/>
       <c r="C5" s="6">
         <v>40</v>
       </c>
       <c r="D5" s="36"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="58"/>
-    </row>
-    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="57"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="57"/>
+    </row>
+    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A6" s="37"/>
-      <c r="B6" s="59"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="6">
         <v>50</v>
       </c>
       <c r="D6" s="37"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="59"/>
-    </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="56">
+      <c r="E6" s="58"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="58"/>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A7" s="71">
         <v>2</v>
       </c>
-      <c r="B7" s="69" t="s">
-        <v>98</v>
+      <c r="B7" s="63" t="s">
+        <v>96</v>
       </c>
       <c r="C7" s="11">
         <v>15</v>
       </c>
       <c r="D7" s="52">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="E7" s="52">
         <v>1</v>
@@ -1887,45 +1887,45 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="56"/>
-      <c r="B8" s="70"/>
+    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A8" s="71"/>
+      <c r="B8" s="64"/>
       <c r="C8" s="11">
         <v>20</v>
       </c>
       <c r="D8" s="53"/>
       <c r="E8" s="53"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
-    </row>
-    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="56"/>
-      <c r="B9" s="70"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="69"/>
+    </row>
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A9" s="71"/>
+      <c r="B9" s="64"/>
       <c r="C9" s="11">
         <v>25</v>
       </c>
       <c r="D9" s="53"/>
       <c r="E9" s="53"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-    </row>
-    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="56"/>
-      <c r="B10" s="71"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+    </row>
+    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A10" s="71"/>
+      <c r="B10" s="65"/>
       <c r="C10" s="11">
         <v>30</v>
       </c>
       <c r="D10" s="54"/>
       <c r="E10" s="54"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-    </row>
-    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="47">
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+    </row>
+    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A11" s="62">
         <v>3</v>
       </c>
-      <c r="B11" s="72" t="s">
-        <v>99</v>
+      <c r="B11" s="66" t="s">
+        <v>97</v>
       </c>
       <c r="C11" s="11">
         <v>50</v>
@@ -1943,51 +1943,51 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="47"/>
-      <c r="B12" s="73"/>
+    <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A12" s="62"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="11">
         <v>75</v>
       </c>
       <c r="D12" s="53"/>
       <c r="E12" s="53"/>
-      <c r="F12" s="63"/>
+      <c r="F12" s="69"/>
       <c r="G12" s="53"/>
     </row>
-    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="47"/>
-      <c r="B13" s="73"/>
+    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A13" s="62"/>
+      <c r="B13" s="67"/>
       <c r="C13" s="11">
         <v>90</v>
       </c>
       <c r="D13" s="53"/>
       <c r="E13" s="53"/>
-      <c r="F13" s="63"/>
+      <c r="F13" s="69"/>
       <c r="G13" s="53"/>
     </row>
-    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="47"/>
-      <c r="B14" s="74"/>
+    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A14" s="62"/>
+      <c r="B14" s="68"/>
       <c r="C14" s="11">
         <v>120</v>
       </c>
       <c r="D14" s="54"/>
       <c r="E14" s="54"/>
-      <c r="F14" s="64"/>
+      <c r="F14" s="70"/>
       <c r="G14" s="54"/>
     </row>
-    <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="47">
+    <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A15" s="62">
         <v>4</v>
       </c>
-      <c r="B15" s="72" t="s">
-        <v>100</v>
+      <c r="B15" s="66" t="s">
+        <v>98</v>
       </c>
       <c r="C15" s="6">
         <v>25</v>
       </c>
       <c r="D15" s="35">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="E15" s="52">
         <v>4</v>
@@ -1999,9 +1999,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="47"/>
-      <c r="B16" s="73"/>
+    <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A16" s="62"/>
+      <c r="B16" s="67"/>
       <c r="C16" s="6">
         <v>35</v>
       </c>
@@ -2010,9 +2010,9 @@
       <c r="F16" s="53"/>
       <c r="G16" s="53"/>
     </row>
-    <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="47"/>
-      <c r="B17" s="73"/>
+    <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A17" s="62"/>
+      <c r="B17" s="67"/>
       <c r="C17" s="6">
         <v>40</v>
       </c>
@@ -2021,9 +2021,9 @@
       <c r="F17" s="53"/>
       <c r="G17" s="53"/>
     </row>
-    <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="47"/>
-      <c r="B18" s="74"/>
+    <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A18" s="62"/>
+      <c r="B18" s="68"/>
       <c r="C18" s="6">
         <v>50</v>
       </c>
@@ -2032,7 +2032,7 @@
       <c r="F18" s="54"/>
       <c r="G18" s="54"/>
     </row>
-    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
@@ -2047,10 +2047,10 @@
       <c r="F20" s="30"/>
       <c r="G20" s="31"/>
       <c r="H20" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A21" s="5" t="s">
         <v>11</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>29</v>
       </c>
       <c r="C22" s="49" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D22" s="50"/>
       <c r="E22" s="50"/>
@@ -2126,28 +2126,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D9C119C-42F6-4CF6-ADF9-8275A6751DB2}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="2" max="2" width="15.625" customWidth="1"/>
     <col min="7" max="7" width="45.625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
-        <v>131</v>
-      </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A3" s="28">
         <v>1</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="35">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="E3" s="35">
         <v>4</v>
@@ -2193,7 +2193,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A4" s="28"/>
       <c r="B4" s="36"/>
       <c r="C4" s="14">
@@ -2204,7 +2204,7 @@
       <c r="F4" s="36"/>
       <c r="G4" s="42"/>
     </row>
-    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="28"/>
       <c r="B5" s="36"/>
       <c r="C5" s="14">
@@ -2215,7 +2215,7 @@
       <c r="F5" s="36"/>
       <c r="G5" s="42"/>
     </row>
-    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A6" s="28"/>
       <c r="B6" s="37"/>
       <c r="C6" s="14">
@@ -2226,7 +2226,7 @@
       <c r="F6" s="37"/>
       <c r="G6" s="43"/>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A7" s="28">
         <v>2</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="35">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="E7" s="35">
         <v>2</v>
@@ -2246,10 +2246,10 @@
         <v>6</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A8" s="28"/>
       <c r="B8" s="36"/>
       <c r="C8" s="14">
@@ -2259,10 +2259,10 @@
       <c r="E8" s="36"/>
       <c r="F8" s="36"/>
       <c r="G8" s="16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A9" s="28"/>
       <c r="B9" s="36"/>
       <c r="C9" s="14">
@@ -2272,10 +2272,10 @@
       <c r="E9" s="36"/>
       <c r="F9" s="36"/>
       <c r="G9" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A10" s="28"/>
       <c r="B10" s="37"/>
       <c r="C10" s="14">
@@ -2285,10 +2285,10 @@
       <c r="E10" s="37"/>
       <c r="F10" s="37"/>
       <c r="G10" s="16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A11" s="28">
         <v>3</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="35">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E11" s="35">
         <v>1</v>
@@ -2308,10 +2308,10 @@
         <v>12</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A12" s="28"/>
       <c r="B12" s="36"/>
       <c r="C12" s="14">
@@ -2323,10 +2323,10 @@
         <v>11</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A13" s="28"/>
       <c r="B13" s="36"/>
       <c r="C13" s="14">
@@ -2338,10 +2338,10 @@
         <v>10</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A14" s="28"/>
       <c r="B14" s="37"/>
       <c r="C14" s="14">
@@ -2353,10 +2353,10 @@
         <v>9</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A15" s="28">
         <v>4</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A16" s="28"/>
       <c r="B16" s="36"/>
       <c r="C16" s="14">
@@ -2390,7 +2390,7 @@
       <c r="F16" s="36"/>
       <c r="G16" s="42"/>
     </row>
-    <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A17" s="28"/>
       <c r="B17" s="36"/>
       <c r="C17" s="14">
@@ -2401,7 +2401,7 @@
       <c r="F17" s="36"/>
       <c r="G17" s="42"/>
     </row>
-    <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A18" s="28"/>
       <c r="B18" s="37"/>
       <c r="C18" s="14">
@@ -2412,7 +2412,7 @@
       <c r="F18" s="37"/>
       <c r="G18" s="43"/>
     </row>
-    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
@@ -2427,41 +2427,41 @@
       <c r="F20" s="30"/>
       <c r="G20" s="31"/>
       <c r="H20" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A21" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="65" t="s">
+      <c r="C21" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="66"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="67"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="74"/>
       <c r="H21" s="13">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="65" t="s">
+      <c r="C22" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="66"/>
-      <c r="E22" s="66"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="67"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="74"/>
       <c r="H22" s="13">
         <v>12</v>
       </c>
@@ -2507,7 +2507,7 @@
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="2" width="15.625" customWidth="1"/>
     <col min="3" max="4" width="8.625" customWidth="1"/>
@@ -2516,58 +2516,58 @@
     <col min="9" max="9" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.6">
       <c r="C1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E2" s="22" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G2" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A3" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
-        <v>56</v>
-      </c>
       <c r="B3" s="22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E3" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="26" t="s">
         <v>105</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>107</v>
       </c>
       <c r="G3" s="26">
         <v>20</v>
@@ -2576,21 +2576,21 @@
         <v>3</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A4" s="21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" s="22" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E4" s="26">
         <v>5</v>
@@ -2602,24 +2602,24 @@
         <v>25</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A5" s="21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E5" s="26">
         <v>1</v>
@@ -2628,33 +2628,33 @@
         <v>10</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A6" s="21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="21" t="s">
-        <v>66</v>
-      </c>
       <c r="D6" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G6" s="26">
         <v>20</v>
@@ -2663,27 +2663,27 @@
         <v>8</v>
       </c>
       <c r="I6" s="21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A7" s="21" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
-        <v>76</v>
-      </c>
       <c r="B7" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C7" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="21" t="s">
         <v>110</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>112</v>
       </c>
       <c r="E7" s="26">
         <v>1</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G7" s="26">
         <v>25</v>
@@ -2692,27 +2692,27 @@
         <v>1</v>
       </c>
       <c r="I7" s="21" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A8" s="21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C8" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="21" t="s">
         <v>110</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>112</v>
       </c>
       <c r="E8" s="26">
         <v>1</v>
       </c>
       <c r="F8" s="26" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G8" s="27">
         <v>15</v>
@@ -2721,56 +2721,56 @@
         <v>11</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A9" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C9" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="D9" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>113</v>
-      </c>
       <c r="F9" s="26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H9" s="26">
         <v>13</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A10" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C10" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="21" t="s">
         <v>110</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>112</v>
       </c>
       <c r="E10" s="26">
         <v>4</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G10" s="26">
         <v>25</v>
@@ -2779,27 +2779,27 @@
         <v>10</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A11" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C11" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="21" t="s">
         <v>110</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>112</v>
       </c>
       <c r="E11" s="27">
         <v>4</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G11" s="26">
         <v>25</v>
@@ -2808,27 +2808,27 @@
         <v>2</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A12" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C12" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="21" t="s">
         <v>110</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>112</v>
       </c>
       <c r="E12" s="26">
         <v>2</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G12" s="26">
         <v>30</v>
@@ -2837,82 +2837,82 @@
         <v>6</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K12" s="25"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A13" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E13" s="26">
         <v>1</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G13" s="26">
         <v>20</v>
       </c>
       <c r="H13" s="26" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K13" s="25"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A14" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H14" s="26">
         <v>12</v>
       </c>
       <c r="I14" s="21" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K14" s="25"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.6">
       <c r="K15" s="25"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A17" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B17" s="22" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D17" s="22" t="s">
         <v>9</v>
@@ -2923,18 +2923,18 @@
       <c r="H17" s="23"/>
       <c r="I17" s="23"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A18" s="22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C18" s="22">
         <v>12</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
@@ -2942,18 +2942,18 @@
       <c r="H18" s="23"/>
       <c r="I18" s="23"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A19" s="22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C19" s="22">
         <v>15</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
@@ -2961,9 +2961,9 @@
       <c r="H19" s="23"/>
       <c r="I19" s="23"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A20" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B20" s="22" t="s">
         <v>28</v>
@@ -2972,7 +2972,7 @@
         <v>20</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E20" s="23"/>
       <c r="F20" s="23"/>
@@ -2980,9 +2980,9 @@
       <c r="H20" s="23"/>
       <c r="I20" s="23"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A21" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B21" s="22" t="s">
         <v>29</v>
@@ -2991,7 +2991,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E21" s="23"/>
       <c r="F21" s="23"/>
@@ -2999,9 +2999,9 @@
       <c r="H21" s="23"/>
       <c r="I21" s="23"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A22" s="22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B22" s="22" t="s">
         <v>14</v>
@@ -3010,7 +3010,7 @@
         <v>12</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E22" s="23"/>
       <c r="F22" s="23"/>
@@ -3018,9 +3018,9 @@
       <c r="H22" s="23"/>
       <c r="I22" s="23"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A23" s="22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B23" s="22" t="s">
         <v>12</v>
@@ -3029,7 +3029,7 @@
         <v>12</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3046,13 +3046,13 @@
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="2" max="2" width="15.625" customWidth="1"/>
     <col min="7" max="7" width="45.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="35">
         <v>1</v>
       </c>
@@ -3086,7 +3086,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A3" s="36"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -3095,7 +3095,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A4" s="36"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -3104,7 +3104,7 @@
       <c r="F4" s="6"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="37"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -3113,8 +3113,8 @@
       <c r="F5" s="6"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="56">
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="71">
         <v>2</v>
       </c>
       <c r="B6" s="2"/>
@@ -3124,8 +3124,8 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="56"/>
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A7" s="71"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -3133,8 +3133,8 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="56"/>
+    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A8" s="71"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -3142,8 +3142,8 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="56"/>
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A9" s="71"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -3151,8 +3151,8 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="47">
+    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A10" s="62">
         <v>3</v>
       </c>
       <c r="B10" s="9"/>
@@ -3162,8 +3162,8 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="47"/>
+    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A11" s="62"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -3171,8 +3171,8 @@
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="47"/>
+    <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A12" s="62"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -3180,8 +3180,8 @@
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="47"/>
+    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A13" s="62"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -3189,8 +3189,8 @@
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="47">
+    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A14" s="62">
         <v>4</v>
       </c>
       <c r="B14" s="9"/>
@@ -3200,8 +3200,8 @@
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="47"/>
+    <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A15" s="62"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -3209,8 +3209,8 @@
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="47"/>
+    <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A16" s="62"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -3218,8 +3218,8 @@
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="47"/>
+    <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A17" s="62"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -3227,7 +3227,7 @@
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A20" s="5" t="s">
         <v>11</v>
       </c>
@@ -3257,7 +3257,7 @@
       <c r="G20" s="34"/>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A21" s="5" t="s">
         <v>10</v>
       </c>

</xml_diff>